<commit_message>
Sum() now works correctly
</commit_message>
<xml_diff>
--- a/ExcelHO/Finanzen 2017_Test.xlsx
+++ b/ExcelHO/Finanzen 2017_Test.xlsx
@@ -43063,10 +43063,13 @@
         <v>29</v>
       </c>
       <c r="C8" s="102">
-        <f>Summe(C19,C41,C46,C47,C54,C55,C61,C62,C70,C81,C91,C94,C96,)</f>
+        <f>SUM(C19,C41,C46,C47,C54,C55,C61,C62,C70,C81,C91,C94,C96,)</f>
         <v/>
       </c>
-      <c r="D8" s="85" t="n"/>
+      <c r="D8" s="85">
+        <f>(C19+C41+C46+C47+C54+C55+C61+C62+C70+C81+C91+C94+C96+)</f>
+        <v/>
+      </c>
       <c r="E8" s="85" t="n"/>
       <c r="F8" s="85" t="n"/>
     </row>

</xml_diff>